<commit_message>
9 - Completando tabela de gerenciamento de tempo com todas as etapas
</commit_message>
<xml_diff>
--- a/docs/2/tabela-gerenciamento-tempo.xlsx
+++ b/docs/2/tabela-gerenciamento-tempo.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
   <si>
     <t>Atividades</t>
   </si>
@@ -22,10 +22,7 @@
     <t>2º Etapa</t>
   </si>
   <si>
-    <t>3º Etapa</t>
-  </si>
-  <si>
-    <t>4º Etapa</t>
+    <t>3º e 4º Etapa</t>
   </si>
   <si>
     <t>5º Etapa</t>
@@ -43,7 +40,7 @@
     <t>4º Semana</t>
   </si>
   <si>
-    <t>5º Semana</t>
+    <t>9º Semana</t>
   </si>
   <si>
     <t>Documentação de Contexto</t>
@@ -59,20 +56,30 @@
   </si>
   <si>
     <t>Projeto de Interface</t>
-  </si>
-  <si>
-    <t>Programação de Funcionalidades</t>
-  </si>
-  <si>
-    <t>Planos de Testes de Funcionalidades e Usabilidade</t>
-  </si>
-  <si>
-    <t>Registros de Testes de Funcionaliadades e Usabilidade</t>
   </si>
   <si>
     <t>Criar tabelas, graficos ou dashboards com no minimo 
 5 indicadores de desempenho e metas para o 
 processo de negócio</t>
+  </si>
+  <si>
+    <t>Programação de Funcionalidades</t>
+  </si>
+  <si>
+    <t>Planos de Testes de Funcionalidades e Usabilidade</t>
+  </si>
+  <si>
+    <t>Registros de Testes de Funcionaliadades e Usabilidade</t>
+  </si>
+  <si>
+    <t>Considerações Finais</t>
+  </si>
+  <si>
+    <t>Entrega de Vídeo de Apresentação Final e PDF usado 
+na Apresentação</t>
+  </si>
+  <si>
+    <t>Realização da Apresentação Final</t>
   </si>
 </sst>
 </file>
@@ -113,6 +120,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFCFE2F3"/>
         <bgColor rgb="FFCFE2F3"/>
       </patternFill>
@@ -123,12 +136,6 @@
         <bgColor rgb="FF3D85C6"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border/>
@@ -136,7 +143,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -147,17 +154,23 @@
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -390,228 +403,223 @@
       <c r="I1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+    </row>
+    <row r="2">
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="I2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="L2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="M2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="5"/>
+        <v>10</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="5"/>
+        <v>11</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
-      <c r="P5" s="5"/>
-      <c r="Q5" s="5"/>
+        <v>12</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="5"/>
-      <c r="Q6" s="5"/>
+        <v>13</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
+        <v>14</v>
+      </c>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
+        <v>15</v>
+      </c>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
+        <v>16</v>
+      </c>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="7"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
+        <v>17</v>
+      </c>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="8"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="8"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="10"/>
     </row>
     <row r="13">
-      <c r="A13" s="8"/>
+      <c r="A13" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10"/>
+      <c r="P13" s="10"/>
     </row>
     <row r="14">
-      <c r="A14" s="8"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="8"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="8"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="8"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="8"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="8"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="8"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="8"/>
+      <c r="A14" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="5">
     <mergeCell ref="A1:A2"/>
-    <mergeCell ref="Q1:S1"/>
-    <mergeCell ref="L1:P1"/>
-    <mergeCell ref="I1:K1"/>
     <mergeCell ref="E1:H1"/>
     <mergeCell ref="B1:D1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:M1"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>